<commit_message>
ALU truth table and equations
</commit_message>
<xml_diff>
--- a/ALU truth table.xlsx
+++ b/ALU truth table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2DCC1A-C195-469A-AB97-1089C315A347}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{538EBF66-6646-4EA6-A49F-0C05CCE20684}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="2595" windowHeight="5775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -640,8 +640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>